<commit_message>
Sprint 2 backlog update
</commit_message>
<xml_diff>
--- a/Documentation/Scrum/Sprint2Backlog.xlsx
+++ b/Documentation/Scrum/Sprint2Backlog.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Ali\Documents\cst247\Documentation\Scrum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caleb Ljunggren\Documents\School (GCU)\CST-247\Bitbucket-GitHub\Documentation\Scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Use Case Template" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>User Stories</t>
   </si>
@@ -89,12 +89,15 @@
   </si>
   <si>
     <t>I can have a better experience</t>
+  </si>
+  <si>
+    <t>Caleb Ljunggren</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -577,11 +580,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,7 +687,7 @@
         <v>4</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>